<commit_message>
tambahkan perhitungan manual excel
</commit_message>
<xml_diff>
--- a/dokumentasi/hitung-manual.xlsx
+++ b/dokumentasi/hitung-manual.xlsx
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,23 +1134,23 @@
         <v>26</v>
       </c>
       <c r="B14" s="8">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="8">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="D14" s="8">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="E14" s="8">
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="F14" s="8">
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="8">
         <f>SUM(B14:F14)</f>
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1222,6 +1222,10 @@
       <c r="F18" s="5">
         <f>F14/G14</f>
         <v>0.2</v>
+      </c>
+      <c r="G18" s="8">
+        <f>SUM(B18:F18)</f>
+        <v>1</v>
       </c>
       <c r="J18" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
ubah perhitungan manual agar signifikan
</commit_message>
<xml_diff>
--- a/dokumentasi/hitung-manual.xlsx
+++ b/dokumentasi/hitung-manual.xlsx
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,7 @@
         <v>50</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -933,7 +933,7 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -991,7 +991,7 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -1143,10 +1143,10 @@
         <v>5</v>
       </c>
       <c r="E14" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="8">
         <f>SUM(B14:F14)</f>
@@ -1217,11 +1217,11 @@
       </c>
       <c r="E18" s="5">
         <f>E14/G14</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F18" s="5">
         <f>F14/G14</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="G18" s="8">
         <f>SUM(B18:F18)</f>
@@ -1287,15 +1287,15 @@
       </c>
       <c r="E22">
         <f>POWER(E4,E18)</f>
-        <v>2.1867241478865562</v>
+        <v>1.7982310843956588</v>
       </c>
       <c r="F22">
         <f>POWER(F4,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22:G31" si="0">(B22*C22*D22*E22*F22)</f>
-        <v>34.968409520721472</v>
+        <v>34.086580994024978</v>
       </c>
       <c r="J22" t="s">
         <v>14</v>
@@ -1322,11 +1322,11 @@
       </c>
       <c r="E23">
         <f>POWER(E5,E18)</f>
-        <v>1.97435048583482</v>
+        <v>1.665590320178459</v>
       </c>
       <c r="F23">
         <f>POWER(F5,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C24">
         <f>POWER(C6,C18)</f>
-        <v>2.514866859365871</v>
+        <v>2.1147425268811282</v>
       </c>
       <c r="D24">
         <f>POWER(D6,D18)</f>
@@ -1357,15 +1357,15 @@
       </c>
       <c r="E24">
         <f>POWER(E6,E18)</f>
-        <v>2.1867241478865562</v>
+        <v>1.7982310843956588</v>
       </c>
       <c r="F24">
         <f>POWER(F6,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>37.576001434659375</v>
+        <v>30.800702882410231</v>
       </c>
       <c r="J24" t="s">
         <v>17</v>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="C25">
         <f>POWER(C7,C18)</f>
-        <v>2.514866859365871</v>
+        <v>2.6591479484724942</v>
       </c>
       <c r="D25">
         <f>POWER(D7,D18)</f>
@@ -1392,15 +1392,15 @@
       </c>
       <c r="E25">
         <f>POWER(E7,E18)</f>
-        <v>1.97435048583482</v>
+        <v>1.665590320178459</v>
       </c>
       <c r="F25">
         <f>POWER(F7,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>33.926637138914693</v>
+        <v>35.873051175863793</v>
       </c>
       <c r="J25" t="s">
         <v>18</v>
@@ -1427,15 +1427,15 @@
       </c>
       <c r="E26">
         <f>POWER(E8,E18)</f>
-        <v>1.97435048583482</v>
+        <v>1.665590320178459</v>
       </c>
       <c r="F26">
         <f>POWER(F8,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>31.572293374467765</v>
+        <v>31.572293374467762</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>25</v>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="C27">
         <f>POWER(C9,C18)</f>
-        <v>1.778279410038923</v>
+        <v>2.6591479484724942</v>
       </c>
       <c r="D27">
         <f>POWER(D9,D18)</f>
@@ -1462,15 +1462,15 @@
       </c>
       <c r="E27">
         <f>POWER(E9,E18)</f>
-        <v>2.1867241478865562</v>
+        <v>1.7982310843956588</v>
       </c>
       <c r="F27">
         <f>POWER(F9,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>26.57024542432308</v>
+        <v>38.729833462074168</v>
       </c>
       <c r="J27" t="s">
         <v>19</v>
@@ -1497,11 +1497,11 @@
       </c>
       <c r="E28">
         <f>POWER(E10,E18)</f>
-        <v>1.97435048583482</v>
+        <v>1.665590320178459</v>
       </c>
       <c r="F28">
         <f>POWER(F10,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -1526,15 +1526,15 @@
       </c>
       <c r="E29">
         <f>POWER(E11,E18)</f>
-        <v>2.1867241478865562</v>
+        <v>1.7982310843956588</v>
       </c>
       <c r="F29">
         <f>POWER(F11,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>37.576001434659375</v>
+        <v>36.628415014847064</v>
       </c>
       <c r="J29" t="s">
         <v>12</v>
@@ -1561,11 +1561,11 @@
       </c>
       <c r="E30">
         <f>POWER(E12,E18)</f>
-        <v>1.97435048583482</v>
+        <v>1.665590320178459</v>
       </c>
       <c r="F30">
         <f>POWER(F12,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -1596,11 +1596,11 @@
       </c>
       <c r="E31">
         <f>POWER(E13,E18)</f>
-        <v>1.97435048583482</v>
+        <v>1.665590320178459</v>
       </c>
       <c r="F31">
         <f>POWER(F13,F18)</f>
-        <v>1.97435048583482</v>
+        <v>2.340347319320716</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="G32">
         <f>SUM(G22:G31)</f>
-        <v>338.33752940706404</v>
+        <v>343.83881798300627</v>
       </c>
       <c r="K32" s="2"/>
     </row>
@@ -1647,13 +1647,13 @@
       </c>
       <c r="B35">
         <f>(G22/G32)</f>
-        <v>0.1033536231762511</v>
+        <v>9.9135348341354693E-2</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E35">
-        <v>0.11839938175399509</v>
+        <v>0.1126395026869489</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1662,13 +1662,13 @@
       </c>
       <c r="B36">
         <f>(G23/G32)</f>
-        <v>8.4320493803107077E-2</v>
+        <v>8.2971398398469648E-2</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E36">
-        <v>0.1101830399749523</v>
+        <v>0.1065278645084726</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1677,13 +1677,13 @@
       </c>
       <c r="B37">
         <f>(G24/G32)</f>
-        <v>0.11106069581022021</v>
+        <v>8.9578899389808023E-2</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E37">
-        <v>0.1081862632471846</v>
+        <v>0.1043310100537769</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1692,13 +1692,13 @@
       </c>
       <c r="B38">
         <f>(G25/G32)</f>
-        <v>0.10027453117119779</v>
+        <v>0.1043310100537769</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E38">
-        <v>0.1081862632471846</v>
+        <v>0.1043310100537769</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1707,13 +1707,13 @@
       </c>
       <c r="B39">
         <f>(G26/G32)</f>
-        <v>9.3315965952101607E-2</v>
+        <v>9.1822946459838559E-2</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39">
-        <v>0.10213730002532963</v>
+        <v>0.1043310100537769</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1722,13 +1722,13 @@
       </c>
       <c r="B40">
         <f>(G27/G32)</f>
-        <v>7.8531771130703087E-2</v>
+        <v>0.1126395026869489</v>
       </c>
       <c r="D40" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E40">
-        <v>9.6595494465195372E-2</v>
+        <v>0.1043310100537769</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1737,13 +1737,13 @@
       </c>
       <c r="B41">
         <f>(G28/G32)</f>
-        <v>0.10602740771539963</v>
+        <v>0.1043310100537769</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41">
-        <v>9.5216000043666912E-2</v>
+        <v>9.9135348341354693E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,13 +1752,13 @@
       </c>
       <c r="B42">
         <f>(G29/G32)</f>
-        <v>0.11106069581022021</v>
+        <v>0.1065278645084726</v>
       </c>
       <c r="D42" t="s">
         <v>51</v>
       </c>
       <c r="E42">
-        <v>9.5216000043666885E-2</v>
+        <v>9.1822946459838559E-2</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1767,13 +1767,13 @@
       </c>
       <c r="B43">
         <f>(G30/G32)</f>
-        <v>0.10602740771539963</v>
+        <v>0.1043310100537769</v>
       </c>
       <c r="D43" t="s">
         <v>49</v>
       </c>
       <c r="E43">
-        <v>8.5813464087307639E-2</v>
+        <v>8.9578899389808023E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1782,18 +1782,18 @@
       </c>
       <c r="B44">
         <f>(G31/G32)</f>
-        <v>0.10602740771539963</v>
+        <v>0.1043310100537769</v>
       </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E44">
-        <v>8.0066793111517029E-2</v>
+        <v>8.2971398398469648E-2</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="D35:E44">
-    <sortCondition descending="1" ref="E35:E44"/>
+    <sortCondition descending="1" ref="E35"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="H1:I1"/>

</xml_diff>

<commit_message>
ubah perhitungan manual dan perhitungan program
</commit_message>
<xml_diff>
--- a/dokumentasi/hitung-manual.xlsx
+++ b/dokumentasi/hitung-manual.xlsx
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,14 +1143,14 @@
         <v>5</v>
       </c>
       <c r="E14" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="8">
         <v>5</v>
       </c>
       <c r="G14" s="8">
         <f>SUM(B14:F14)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1205,23 +1205,23 @@
       <c r="A18" s="6"/>
       <c r="B18" s="5">
         <f>B14/G14</f>
-        <v>0.1</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="C18" s="5">
         <f>C14/G14</f>
-        <v>0.25</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="D18" s="5">
         <f>D14/G14</f>
-        <v>0.25</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="E18" s="5">
         <f>E14/G14</f>
-        <v>0.15</v>
+        <v>0.19047619047619047</v>
       </c>
       <c r="F18" s="5">
         <f>F14/G14</f>
-        <v>0.25</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="G18" s="8">
         <f>SUM(B18:F18)</f>
@@ -1275,27 +1275,27 @@
       </c>
       <c r="B22">
         <f>POWER(B4, B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C22">
         <f>POWER(C4,C18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="D22">
         <f>POWER(D4,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E22">
         <f>POWER(E4,E18)</f>
-        <v>1.7982310843956588</v>
+        <v>2.1067516084175355</v>
       </c>
       <c r="F22">
         <f>POWER(F4,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22:G31" si="0">(B22*C22*D22*E22*F22)</f>
-        <v>34.086580994024978</v>
+        <v>34.71415607735252</v>
       </c>
       <c r="J22" t="s">
         <v>14</v>
@@ -1310,27 +1310,27 @@
       </c>
       <c r="B23">
         <f>POWER(B5,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C23">
         <f>POWER(C5,C18)</f>
-        <v>2.1147425268811282</v>
+        <v>2.0406524577302751</v>
       </c>
       <c r="D23">
         <f>POWER(D5,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E23">
         <f>POWER(E5,E18)</f>
-        <v>1.665590320178459</v>
+        <v>1.9114213360578527</v>
       </c>
       <c r="F23">
         <f>POWER(F5,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>28.528787551726904</v>
+        <v>28.597180516131836</v>
       </c>
       <c r="J23" t="s">
         <v>16</v>
@@ -1345,27 +1345,27 @@
       </c>
       <c r="B24">
         <f>POWER(B6,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C24">
         <f>POWER(C6,C18)</f>
-        <v>2.1147425268811282</v>
+        <v>2.0406524577302751</v>
       </c>
       <c r="D24">
         <f>POWER(D6,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E24">
         <f>POWER(E6,E18)</f>
-        <v>1.7982310843956588</v>
+        <v>2.1067516084175355</v>
       </c>
       <c r="F24">
         <f>POWER(F6,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>30.800702882410231</v>
+        <v>31.519558201030705</v>
       </c>
       <c r="J24" t="s">
         <v>17</v>
@@ -1380,27 +1380,27 @@
       </c>
       <c r="B25">
         <f>POWER(B7,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C25">
         <f>POWER(C7,C18)</f>
-        <v>2.6591479484724942</v>
+        <v>2.5381463950956666</v>
       </c>
       <c r="D25">
         <f>POWER(D7,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E25">
         <f>POWER(E7,E18)</f>
-        <v>1.665590320178459</v>
+        <v>1.9114213360578527</v>
       </c>
       <c r="F25">
         <f>POWER(F7,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>35.873051175863793</v>
+        <v>35.568933044900618</v>
       </c>
       <c r="J25" t="s">
         <v>18</v>
@@ -1415,27 +1415,27 @@
       </c>
       <c r="B26">
         <f>POWER(B8,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C26">
         <f>POWER(C8,C18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="D26">
         <f>POWER(D8,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E26">
         <f>POWER(E8,E18)</f>
-        <v>1.665590320178459</v>
+        <v>1.9114213360578527</v>
       </c>
       <c r="F26">
         <f>POWER(F8,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>31.572293374467762</v>
+        <v>31.495587009108601</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>25</v>
@@ -1450,27 +1450,27 @@
       </c>
       <c r="B27">
         <f>POWER(B9,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C27">
         <f>POWER(C9,C18)</f>
-        <v>2.6591479484724942</v>
+        <v>2.5381463950956666</v>
       </c>
       <c r="D27">
         <f>POWER(D9,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E27">
         <f>POWER(E9,E18)</f>
-        <v>1.7982310843956588</v>
+        <v>2.1067516084175355</v>
       </c>
       <c r="F27">
         <f>POWER(F9,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>38.729833462074168</v>
+        <v>39.203761875226853</v>
       </c>
       <c r="J27" t="s">
         <v>19</v>
@@ -1485,27 +1485,27 @@
       </c>
       <c r="B28">
         <f>POWER(B10,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C28">
         <f>POWER(C10,C18)</f>
-        <v>2.6591479484724942</v>
+        <v>2.5381463950956666</v>
       </c>
       <c r="D28">
         <f>POWER(D10,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E28">
         <f>POWER(E10,E18)</f>
-        <v>1.665590320178459</v>
+        <v>1.9114213360578527</v>
       </c>
       <c r="F28">
         <f>POWER(F10,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>35.873051175863793</v>
+        <v>35.568933044900618</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1514,27 +1514,27 @@
       </c>
       <c r="B29">
         <f>POWER(B11,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C29">
         <f>POWER(C11,C18)</f>
-        <v>2.514866859365871</v>
+        <v>2.4068158068741594</v>
       </c>
       <c r="D29">
         <f>POWER(D11,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E29">
         <f>POWER(E11,E18)</f>
-        <v>1.7982310843956588</v>
+        <v>2.1067516084175355</v>
       </c>
       <c r="F29">
         <f>POWER(F11,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>36.628415014847064</v>
+        <v>37.175252756321058</v>
       </c>
       <c r="J29" t="s">
         <v>12</v>
@@ -1549,27 +1549,27 @@
       </c>
       <c r="B30">
         <f>POWER(B12,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C30">
         <f>POWER(C12,C18)</f>
-        <v>2.6591479484724942</v>
+        <v>2.5381463950956666</v>
       </c>
       <c r="D30">
         <f>POWER(D12,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E30">
         <f>POWER(E12,E18)</f>
-        <v>1.665590320178459</v>
+        <v>1.9114213360578527</v>
       </c>
       <c r="F30">
         <f>POWER(F12,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>35.873051175863793</v>
+        <v>35.568933044900618</v>
       </c>
       <c r="J30" t="s">
         <v>79</v>
@@ -1584,27 +1584,27 @@
       </c>
       <c r="B31">
         <f>POWER(B13,B18)</f>
-        <v>1.4787576366283137</v>
+        <v>1.4514653314556072</v>
       </c>
       <c r="C31">
         <f>POWER(C13,C18)</f>
-        <v>2.6591479484724942</v>
+        <v>2.5381463950956666</v>
       </c>
       <c r="D31">
         <f>POWER(D13,D18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="E31">
         <f>POWER(E13,E18)</f>
-        <v>1.665590320178459</v>
+        <v>1.9114213360578527</v>
       </c>
       <c r="F31">
         <f>POWER(F13,F18)</f>
-        <v>2.340347319320716</v>
+        <v>2.2474784533929575</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>35.873051175863793</v>
+        <v>35.568933044900618</v>
       </c>
       <c r="J31" t="s">
         <v>80</v>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="G32">
         <f>SUM(G22:G31)</f>
-        <v>343.83881798300627</v>
+        <v>344.98122861477407</v>
       </c>
       <c r="K32" s="2"/>
     </row>
@@ -1647,13 +1647,13 @@
       </c>
       <c r="B35">
         <f>(G22/G32)</f>
-        <v>9.9135348341354693E-2</v>
+        <v>0.10062621730678671</v>
       </c>
       <c r="D35" t="s">
         <v>52</v>
       </c>
       <c r="E35">
-        <v>0.1126395026869489</v>
+        <v>0.11364027553801785</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1662,13 +1662,13 @@
       </c>
       <c r="B36">
         <f>(G23/G32)</f>
-        <v>8.2971398398469648E-2</v>
+        <v>8.2894888602953798E-2</v>
       </c>
       <c r="D36" t="s">
         <v>54</v>
       </c>
       <c r="E36">
-        <v>0.1065278645084726</v>
+        <v>0.10776021902870862</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1677,13 +1677,13 @@
       </c>
       <c r="B37">
         <f>(G24/G32)</f>
-        <v>8.9578899389808023E-2</v>
+        <v>9.1366009471278389E-2</v>
       </c>
       <c r="D37" t="s">
         <v>50</v>
       </c>
       <c r="E37">
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1692,13 +1692,13 @@
       </c>
       <c r="B38">
         <f>(G25/G32)</f>
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
       <c r="D38" t="s">
         <v>53</v>
       </c>
       <c r="E38">
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1707,13 +1707,13 @@
       </c>
       <c r="B39">
         <f>(G26/G32)</f>
-        <v>9.1822946459838559E-2</v>
+        <v>9.1296523974869342E-2</v>
       </c>
       <c r="D39" t="s">
         <v>55</v>
       </c>
       <c r="E39">
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1722,13 +1722,13 @@
       </c>
       <c r="B40">
         <f>(G27/G32)</f>
-        <v>0.1126395026869489</v>
+        <v>0.11364027553801785</v>
       </c>
       <c r="D40" t="s">
         <v>56</v>
       </c>
       <c r="E40">
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1737,13 +1737,13 @@
       </c>
       <c r="B41">
         <f>(G28/G32)</f>
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
       <c r="D41" t="s">
         <v>47</v>
       </c>
       <c r="E41">
-        <v>9.9135348341354693E-2</v>
+        <v>0.10062621730678671</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,13 +1752,13 @@
       </c>
       <c r="B42">
         <f>(G29/G32)</f>
-        <v>0.1065278645084726</v>
+        <v>0.10776021902870862</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E42">
-        <v>9.1822946459838559E-2</v>
+        <v>9.1366009471278389E-2</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1767,13 +1767,13 @@
       </c>
       <c r="B43">
         <f>(G30/G32)</f>
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E43">
-        <v>8.9578899389808023E-2</v>
+        <v>9.1296523974869342E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1782,13 +1782,13 @@
       </c>
       <c r="B44">
         <f>(G31/G32)</f>
-        <v>0.1043310100537769</v>
+        <v>0.10310396651934631</v>
       </c>
       <c r="D44" t="s">
         <v>48</v>
       </c>
       <c r="E44">
-        <v>8.2971398398469648E-2</v>
+        <v>8.2894888602953798E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cek perhitungan manual dengan aplikasi: sesuai
</commit_message>
<xml_diff>
--- a/dokumentasi/hitung-manual.xlsx
+++ b/dokumentasi/hitung-manual.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="92">
   <si>
     <t>metode diskusi</t>
   </si>
@@ -228,21 +228,6 @@
     <t>A10</t>
   </si>
   <si>
-    <t>pkt1</t>
-  </si>
-  <si>
-    <t>pkt2</t>
-  </si>
-  <si>
-    <t>pkt3</t>
-  </si>
-  <si>
-    <t>pkt4</t>
-  </si>
-  <si>
-    <t>pkt5</t>
-  </si>
-  <si>
     <t>Alternatif</t>
   </si>
   <si>
@@ -286,6 +271,27 @@
   </si>
   <si>
     <t>50.00</t>
+  </si>
+  <si>
+    <t>Kondisi Kelas</t>
+  </si>
+  <si>
+    <t>kondisi Sekolah</t>
+  </si>
+  <si>
+    <t>aktif</t>
+  </si>
+  <si>
+    <t>kondusif</t>
+  </si>
+  <si>
+    <t>cukup kondusif</t>
+  </si>
+  <si>
+    <t>sepi</t>
+  </si>
+  <si>
+    <t>gaduh</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -440,6 +446,12 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -748,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,48 +771,51 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="19"/>
-      <c r="L1" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="21"/>
+      <c r="N1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="H2" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="20"/>
+      <c r="J2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -808,7 +823,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -816,20 +831,23 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>2.0833333333333335</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -848,20 +866,23 @@
       <c r="F4">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="K4" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -880,20 +901,23 @@
       <c r="F5">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>1.25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -912,20 +936,23 @@
       <c r="F6">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -944,20 +971,23 @@
       <c r="F7">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="K7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -976,14 +1006,17 @@
       <c r="F8">
         <v>30</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1002,18 +1035,21 @@
       <c r="F9">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="K9" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1032,20 +1068,23 @@
       <c r="F10">
         <v>30</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="K10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>20</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1064,20 +1103,23 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="H11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="16" t="s">
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="J11" t="s">
-        <v>82</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1096,14 +1138,17 @@
       <c r="F12">
         <v>30</v>
       </c>
-      <c r="J12" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="L12" t="s">
+        <v>79</v>
+      </c>
+      <c r="M12" s="1">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1122,14 +1167,17 @@
       <c r="F13">
         <v>30</v>
       </c>
-      <c r="J13" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="1">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1149,35 +1197,40 @@
         <v>5</v>
       </c>
       <c r="G14" s="8">
-        <f>SUM(B14:F14)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="8">
+        <f>SUM(B14:G14)</f>
+        <v>26</v>
+      </c>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
         <v>24</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="J16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="19"/>
+      <c r="L16" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="10" t="s">
         <v>37</v>
@@ -1194,439 +1247,559 @@
       <c r="F17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J17" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G17" s="10"/>
+      <c r="L17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="5">
-        <f>B14/G14</f>
-        <v>9.5238095238095233E-2</v>
+        <f>B14/H14</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="C18" s="5">
-        <f>C14/G14</f>
-        <v>0.23809523809523808</v>
+        <f>C14/H14</f>
+        <v>0.19230769230769232</v>
       </c>
       <c r="D18" s="5">
-        <f>D14/G14</f>
-        <v>0.23809523809523808</v>
+        <f>D14/H14</f>
+        <v>0.19230769230769232</v>
       </c>
       <c r="E18" s="5">
-        <f>E14/G14</f>
-        <v>0.19047619047619047</v>
+        <f>E14/H14</f>
+        <v>0.15384615384615385</v>
       </c>
       <c r="F18" s="5">
-        <f>F14/G14</f>
-        <v>0.23809523809523808</v>
-      </c>
-      <c r="G18" s="8">
-        <f>SUM(B18:F18)</f>
+        <f>F14/H14</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="G18" s="5">
+        <f>G14/H14</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="H18" s="8">
+        <f>SUM(B18:G18)</f>
         <v>1</v>
       </c>
-      <c r="J18" t="s">
-        <v>87</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="I18" s="8"/>
+      <c r="L18" t="s">
+        <v>82</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="20"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="21"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22">
         <f>POWER(B4, B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C22">
         <f>POWER(C4,C18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="D22">
         <f>POWER(D4,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E22">
         <f>POWER(E4,E18)</f>
-        <v>2.1067516084175355</v>
+        <v>1.8254922800301963</v>
       </c>
       <c r="F22">
         <f>POWER(F4,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:G31" si="0">(B22*C22*D22*E22*F22)</f>
-        <v>34.71415607735252</v>
+        <f>POWER(G4,G18)</f>
+        <v>2.1219004301103888</v>
+      </c>
+      <c r="H22">
+        <f>(B22*C22*D22*E22*F22*G22)</f>
+        <v>37.237484984149461</v>
       </c>
       <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" t="s">
         <v>14</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
         <f>POWER(B5,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C23">
         <f>POWER(C5,C18)</f>
-        <v>2.0406524577302751</v>
+        <v>1.7790906452325863</v>
       </c>
       <c r="D23">
         <f>POWER(D5,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E23">
         <f>POWER(E5,E18)</f>
-        <v>1.9114213360578527</v>
+        <v>1.6875219239328012</v>
       </c>
       <c r="F23">
         <f>POWER(F5,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
-        <v>28.597180516131836</v>
+        <f>POWER(G5,G18)</f>
+        <v>2.0327710165403481</v>
+      </c>
+      <c r="H23">
+        <f>(B23*C23*D23*E23*F23*G23)</f>
+        <v>30.503489186673839</v>
       </c>
       <c r="J23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="2">
-        <v>2.0833333333333335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
         <f>POWER(B6,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C24">
         <f>POWER(C6,C18)</f>
-        <v>2.0406524577302751</v>
+        <v>1.7790906452325863</v>
       </c>
       <c r="D24">
         <f>POWER(D6,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E24">
         <f>POWER(E6,E18)</f>
-        <v>2.1067516084175355</v>
+        <v>1.8254922800301963</v>
       </c>
       <c r="F24">
         <f>POWER(F6,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
-        <v>31.519558201030705</v>
+        <f>POWER(G6,G18)</f>
+        <v>1.9233653142060292</v>
+      </c>
+      <c r="H24">
+        <f>(B24*C24*D24*E24*F24*G24)</f>
+        <v>31.221474979314983</v>
       </c>
       <c r="J24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="2">
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
         <f>POWER(B7,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C25">
         <f>POWER(C7,C18)</f>
-        <v>2.5381463950956666</v>
+        <v>2.1219004301103888</v>
       </c>
       <c r="D25">
         <f>POWER(D7,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E25">
         <f>POWER(E7,E18)</f>
-        <v>1.9114213360578527</v>
+        <v>1.6875219239328012</v>
       </c>
       <c r="F25">
         <f>POWER(F7,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>35.568933044900618</v>
+        <f>POWER(G7,G18)</f>
+        <v>2.1219004301103888</v>
+      </c>
+      <c r="H25">
+        <f>(B25*C25*D25*E25*F25*G25)</f>
+        <v>37.976329364257886</v>
       </c>
       <c r="J25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="2">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26">
         <f>POWER(B8,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C26">
         <f>POWER(C8,C18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="D26">
         <f>POWER(D8,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E26">
         <f>POWER(E8,E18)</f>
-        <v>1.9114213360578527</v>
+        <v>1.6875219239328012</v>
       </c>
       <c r="F26">
         <f>POWER(F8,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
-        <v>31.495587009108601</v>
-      </c>
-      <c r="J26" s="3" t="s">
+        <f>POWER(G8,G18)</f>
+        <v>1.9233653142060292</v>
+      </c>
+      <c r="H26">
+        <f>(B26*C26*D26*E26*F26*G26)</f>
+        <v>31.202295331083668</v>
+      </c>
+      <c r="J26" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K26" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
       <c r="B27">
         <f>POWER(B9,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C27">
         <f>POWER(C9,C18)</f>
-        <v>2.5381463950956666</v>
+        <v>2.1219004301103888</v>
       </c>
       <c r="D27">
         <f>POWER(D9,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E27">
         <f>POWER(E9,E18)</f>
-        <v>2.1067516084175355</v>
+        <v>1.8254922800301963</v>
       </c>
       <c r="F27">
         <f>POWER(F9,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
-        <v>39.203761875226853</v>
+        <f>POWER(G9,G18)</f>
+        <v>2.0327710165403481</v>
+      </c>
+      <c r="H27">
+        <f>(B27*C27*D27*E27*F27*G27)</f>
+        <v>39.35564380076319</v>
       </c>
       <c r="J27" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28">
         <f>POWER(B10,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C28">
         <f>POWER(C10,C18)</f>
-        <v>2.5381463950956666</v>
+        <v>2.1219004301103888</v>
       </c>
       <c r="D28">
         <f>POWER(D10,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E28">
         <f>POWER(E10,E18)</f>
-        <v>1.9114213360578527</v>
+        <v>1.6875219239328012</v>
       </c>
       <c r="F28">
         <f>POWER(F10,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
-        <v>35.568933044900618</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <f>POWER(G10,G18)</f>
+        <v>1.5570684047537311</v>
+      </c>
+      <c r="H28">
+        <f>(B28*C28*D28*E28*F28*G28)</f>
+        <v>27.86735029717255</v>
+      </c>
+      <c r="J28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29">
         <f>POWER(B11,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C29">
         <f>POWER(C11,C18)</f>
-        <v>2.4068158068741594</v>
+        <v>2.0327710165403481</v>
       </c>
       <c r="D29">
         <f>POWER(D11,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E29">
         <f>POWER(E11,E18)</f>
-        <v>2.1067516084175355</v>
+        <v>1.8254922800301963</v>
       </c>
       <c r="F29">
         <f>POWER(F11,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
-        <v>37.175252756321058</v>
+        <f>POWER(G11,G18)</f>
+        <v>1.5570684047537311</v>
+      </c>
+      <c r="H29">
+        <f>(B29*C29*D29*E29*F29*G29)</f>
+        <v>28.879502846286915</v>
       </c>
       <c r="J29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" t="s">
         <v>12</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30">
         <f>POWER(B12,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C30">
         <f>POWER(C12,C18)</f>
-        <v>2.5381463950956666</v>
+        <v>2.1219004301103888</v>
       </c>
       <c r="D30">
         <f>POWER(D12,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E30">
         <f>POWER(E12,E18)</f>
-        <v>1.9114213360578527</v>
+        <v>1.6875219239328012</v>
       </c>
       <c r="F30">
         <f>POWER(F12,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
-        <v>35.568933044900618</v>
+        <f>POWER(G12,G18)</f>
+        <v>1.7790906452325863</v>
+      </c>
+      <c r="H30">
+        <f>(B30*C30*D30*E30*F30*G30)</f>
+        <v>31.840953210376558</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31">
         <f>POWER(B13,B18)</f>
-        <v>1.4514653314556072</v>
+        <v>1.3511077973389822</v>
       </c>
       <c r="C31">
         <f>POWER(C13,C18)</f>
-        <v>2.5381463950956666</v>
+        <v>2.1219004301103888</v>
       </c>
       <c r="D31">
         <f>POWER(D13,D18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="E31">
         <f>POWER(E13,E18)</f>
-        <v>1.9114213360578527</v>
+        <v>1.6875219239328012</v>
       </c>
       <c r="F31">
         <f>POWER(F13,F18)</f>
-        <v>2.2474784533929575</v>
+        <v>1.9233653142060292</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
-        <v>35.568933044900618</v>
+        <f>POWER(G13,G18)</f>
+        <v>1.9233653142060292</v>
+      </c>
+      <c r="H31">
+        <f>(B31*C31*D31*E31*F31*G31)</f>
+        <v>34.423083017273157</v>
       </c>
       <c r="J31" t="s">
-        <v>80</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F32" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G32">
-        <f>SUM(G22:G31)</f>
-        <v>344.98122861477407</v>
-      </c>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G32" s="7"/>
+      <c r="H32">
+        <f>SUM(H22:H31)</f>
+        <v>330.5076070173522</v>
+      </c>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -1639,167 +1812,262 @@
       <c r="E34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K34" s="21"/>
+      <c r="L34" t="s">
+        <v>87</v>
+      </c>
+      <c r="M34" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
       <c r="B35">
-        <f>(G22/G32)</f>
-        <v>0.10062621730678671</v>
+        <f>(H22/H32)</f>
+        <v>0.1126675580032699</v>
       </c>
       <c r="D35" t="s">
         <v>52</v>
       </c>
       <c r="E35">
-        <v>0.11364027553801785</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.11907636304025206</v>
+      </c>
+      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" t="s">
+        <v>88</v>
+      </c>
+      <c r="M35" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
       <c r="B36">
-        <f>(G23/G32)</f>
-        <v>8.2894888602953798E-2</v>
+        <f>(H23/H32)</f>
+        <v>9.2292850569918511E-2</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E36">
-        <v>0.10776021902870862</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.11490304173926037</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L36" t="s">
+        <v>89</v>
+      </c>
+      <c r="M36" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>49</v>
       </c>
       <c r="B37">
-        <f>(G24/G32)</f>
-        <v>9.1366009471278389E-2</v>
+        <f>(H24/H32)</f>
+        <v>9.4465223542270257E-2</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E37">
-        <v>0.10310396651934631</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.1126675580032699</v>
+      </c>
+      <c r="J37" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L37" t="s">
+        <v>90</v>
+      </c>
+      <c r="M37" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>50</v>
       </c>
       <c r="B38">
-        <f>(G25/G32)</f>
-        <v>0.10310396651934631</v>
+        <f>(H25/H32)</f>
+        <v>0.11490304173926037</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E38">
-        <v>0.10310396651934631</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.10415216559740451</v>
+      </c>
+      <c r="J38" t="s">
+        <v>3</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L38" t="s">
+        <v>91</v>
+      </c>
+      <c r="M38" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
       <c r="B39">
-        <f>(G26/G32)</f>
-        <v>9.1296523974869342E-2</v>
+        <f>(H26/H32)</f>
+        <v>9.440719265939769E-2</v>
       </c>
       <c r="D39" t="s">
         <v>55</v>
       </c>
       <c r="E39">
-        <v>0.10310396651934631</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.6339547212614854E-2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
       <c r="B40">
-        <f>(G27/G32)</f>
-        <v>0.11364027553801785</v>
+        <f>(H27/H32)</f>
+        <v>0.11907636304025206</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E40">
-        <v>0.10310396651934631</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.4465223542270257E-2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
       <c r="B41">
-        <f>(G28/G32)</f>
-        <v>0.10310396651934631</v>
+        <f>(H28/H32)</f>
+        <v>8.4316819660097769E-2</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E41">
-        <v>0.10062621730678671</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.440719265939769E-2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>54</v>
       </c>
       <c r="B42">
-        <f>(G29/G32)</f>
-        <v>0.10776021902870862</v>
+        <f>(H29/H32)</f>
+        <v>8.7379237975514112E-2</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42">
-        <v>9.1366009471278389E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.2292850569918511E-2</v>
+      </c>
+      <c r="J42" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
       <c r="B43">
-        <f>(G30/G32)</f>
-        <v>0.10310396651934631</v>
+        <f>(H30/H32)</f>
+        <v>9.6339547212614854E-2</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E43">
-        <v>9.1296523974869342E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.7379237975514112E-2</v>
+      </c>
+      <c r="J43" t="s">
+        <v>8</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>56</v>
       </c>
       <c r="B44">
-        <f>(G31/G32)</f>
-        <v>0.10310396651934631</v>
+        <f>(H31/H32)</f>
+        <v>0.10415216559740451</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E44">
-        <v>8.2894888602953798E-2</v>
+        <v>8.4316819660097769E-2</v>
+      </c>
+      <c r="J44" t="s">
+        <v>83</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="D35:E44">
     <sortCondition descending="1" ref="E35"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="H1:I1"/>
+  <mergeCells count="6">
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A20:H20"/>
     <mergeCell ref="A16:F16"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing bugs session management
</commit_message>
<xml_diff>
--- a/dokumentasi/hitung-manual.xlsx
+++ b/dokumentasi/hitung-manual.xlsx
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1367,7 @@
         <v>2.1219004301103888</v>
       </c>
       <c r="H22">
-        <f>(B22*C22*D22*E22*F22*G22)</f>
+        <f t="shared" ref="H22:H31" si="0">(B22*C22*D22*E22*F22*G22)</f>
         <v>37.237484984149461</v>
       </c>
       <c r="J22" t="s">
@@ -1388,31 +1388,31 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <f>POWER(B5,B18)</f>
+        <f t="shared" ref="B23:G23" si="1">POWER(B5,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C23">
-        <f>POWER(C5,C18)</f>
+        <f t="shared" si="1"/>
         <v>1.7790906452325863</v>
       </c>
       <c r="D23">
-        <f>POWER(D5,D18)</f>
+        <f t="shared" si="1"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E23">
-        <f>POWER(E5,E18)</f>
+        <f t="shared" si="1"/>
         <v>1.6875219239328012</v>
       </c>
       <c r="F23">
-        <f>POWER(F5,F18)</f>
+        <f t="shared" si="1"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G23">
-        <f>POWER(G5,G18)</f>
+        <f t="shared" si="1"/>
         <v>2.0327710165403481</v>
       </c>
       <c r="H23">
-        <f>(B23*C23*D23*E23*F23*G23)</f>
+        <f t="shared" si="0"/>
         <v>30.503489186673839</v>
       </c>
       <c r="J23" t="s">
@@ -1433,31 +1433,31 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <f>POWER(B6,B18)</f>
+        <f t="shared" ref="B24:G24" si="2">POWER(B6,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C24">
-        <f>POWER(C6,C18)</f>
+        <f t="shared" si="2"/>
         <v>1.7790906452325863</v>
       </c>
       <c r="D24">
-        <f>POWER(D6,D18)</f>
+        <f t="shared" si="2"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E24">
-        <f>POWER(E6,E18)</f>
+        <f t="shared" si="2"/>
         <v>1.8254922800301963</v>
       </c>
       <c r="F24">
-        <f>POWER(F6,F18)</f>
+        <f t="shared" si="2"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G24">
-        <f>POWER(G6,G18)</f>
+        <f t="shared" si="2"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="H24">
-        <f>(B24*C24*D24*E24*F24*G24)</f>
+        <f t="shared" si="0"/>
         <v>31.221474979314983</v>
       </c>
       <c r="J24" t="s">
@@ -1478,31 +1478,31 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <f>POWER(B7,B18)</f>
+        <f t="shared" ref="B25:G25" si="3">POWER(B7,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C25">
-        <f>POWER(C7,C18)</f>
+        <f t="shared" si="3"/>
         <v>2.1219004301103888</v>
       </c>
       <c r="D25">
-        <f>POWER(D7,D18)</f>
+        <f t="shared" si="3"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E25">
-        <f>POWER(E7,E18)</f>
+        <f t="shared" si="3"/>
         <v>1.6875219239328012</v>
       </c>
       <c r="F25">
-        <f>POWER(F7,F18)</f>
+        <f t="shared" si="3"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G25">
-        <f>POWER(G7,G18)</f>
+        <f t="shared" si="3"/>
         <v>2.1219004301103888</v>
       </c>
       <c r="H25">
-        <f>(B25*C25*D25*E25*F25*G25)</f>
+        <f t="shared" si="0"/>
         <v>37.976329364257886</v>
       </c>
       <c r="J25" t="s">
@@ -1523,31 +1523,31 @@
         <v>31</v>
       </c>
       <c r="B26">
-        <f>POWER(B8,B18)</f>
+        <f t="shared" ref="B26:G26" si="4">POWER(B8,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C26">
-        <f>POWER(C8,C18)</f>
+        <f t="shared" si="4"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="D26">
-        <f>POWER(D8,D18)</f>
+        <f t="shared" si="4"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E26">
-        <f>POWER(E8,E18)</f>
+        <f t="shared" si="4"/>
         <v>1.6875219239328012</v>
       </c>
       <c r="F26">
-        <f>POWER(F8,F18)</f>
+        <f t="shared" si="4"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G26">
-        <f>POWER(G8,G18)</f>
+        <f t="shared" si="4"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="H26">
-        <f>(B26*C26*D26*E26*F26*G26)</f>
+        <f t="shared" si="0"/>
         <v>31.202295331083668</v>
       </c>
       <c r="J26" t="s">
@@ -1568,31 +1568,31 @@
         <v>57</v>
       </c>
       <c r="B27">
-        <f>POWER(B9,B18)</f>
+        <f t="shared" ref="B27:G27" si="5">POWER(B9,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C27">
-        <f>POWER(C9,C18)</f>
+        <f t="shared" si="5"/>
         <v>2.1219004301103888</v>
       </c>
       <c r="D27">
-        <f>POWER(D9,D18)</f>
+        <f t="shared" si="5"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E27">
-        <f>POWER(E9,E18)</f>
+        <f t="shared" si="5"/>
         <v>1.8254922800301963</v>
       </c>
       <c r="F27">
-        <f>POWER(F9,F18)</f>
+        <f t="shared" si="5"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G27">
-        <f>POWER(G9,G18)</f>
+        <f t="shared" si="5"/>
         <v>2.0327710165403481</v>
       </c>
       <c r="H27">
-        <f>(B27*C27*D27*E27*F27*G27)</f>
+        <f t="shared" si="0"/>
         <v>39.35564380076319</v>
       </c>
       <c r="J27" t="s">
@@ -1613,31 +1613,31 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <f>POWER(B10,B18)</f>
+        <f t="shared" ref="B28:G28" si="6">POWER(B10,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C28">
-        <f>POWER(C10,C18)</f>
+        <f t="shared" si="6"/>
         <v>2.1219004301103888</v>
       </c>
       <c r="D28">
-        <f>POWER(D10,D18)</f>
+        <f t="shared" si="6"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E28">
-        <f>POWER(E10,E18)</f>
+        <f t="shared" si="6"/>
         <v>1.6875219239328012</v>
       </c>
       <c r="F28">
-        <f>POWER(F10,F18)</f>
+        <f t="shared" si="6"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G28">
-        <f>POWER(G10,G18)</f>
+        <f t="shared" si="6"/>
         <v>1.5570684047537311</v>
       </c>
       <c r="H28">
-        <f>(B28*C28*D28*E28*F28*G28)</f>
+        <f t="shared" si="0"/>
         <v>27.86735029717255</v>
       </c>
       <c r="J28" t="s">
@@ -1652,31 +1652,31 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <f>POWER(B11,B18)</f>
+        <f t="shared" ref="B29:G29" si="7">POWER(B11,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C29">
-        <f>POWER(C11,C18)</f>
+        <f t="shared" si="7"/>
         <v>2.0327710165403481</v>
       </c>
       <c r="D29">
-        <f>POWER(D11,D18)</f>
+        <f t="shared" si="7"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E29">
-        <f>POWER(E11,E18)</f>
+        <f t="shared" si="7"/>
         <v>1.8254922800301963</v>
       </c>
       <c r="F29">
-        <f>POWER(F11,F18)</f>
+        <f t="shared" si="7"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G29">
-        <f>POWER(G11,G18)</f>
+        <f t="shared" si="7"/>
         <v>1.5570684047537311</v>
       </c>
       <c r="H29">
-        <f>(B29*C29*D29*E29*F29*G29)</f>
+        <f t="shared" si="0"/>
         <v>28.879502846286915</v>
       </c>
       <c r="J29" t="s">
@@ -1697,31 +1697,31 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <f>POWER(B12,B18)</f>
+        <f t="shared" ref="B30:G30" si="8">POWER(B12,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C30">
-        <f>POWER(C12,C18)</f>
+        <f t="shared" si="8"/>
         <v>2.1219004301103888</v>
       </c>
       <c r="D30">
-        <f>POWER(D12,D18)</f>
+        <f t="shared" si="8"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E30">
-        <f>POWER(E12,E18)</f>
+        <f t="shared" si="8"/>
         <v>1.6875219239328012</v>
       </c>
       <c r="F30">
-        <f>POWER(F12,F18)</f>
+        <f t="shared" si="8"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G30">
-        <f>POWER(G12,G18)</f>
+        <f t="shared" si="8"/>
         <v>1.7790906452325863</v>
       </c>
       <c r="H30">
-        <f>(B30*C30*D30*E30*F30*G30)</f>
+        <f t="shared" si="0"/>
         <v>31.840953210376558</v>
       </c>
       <c r="J30" t="s">
@@ -1742,31 +1742,31 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <f>POWER(B13,B18)</f>
+        <f t="shared" ref="B31:G31" si="9">POWER(B13,B18)</f>
         <v>1.3511077973389822</v>
       </c>
       <c r="C31">
-        <f>POWER(C13,C18)</f>
+        <f t="shared" si="9"/>
         <v>2.1219004301103888</v>
       </c>
       <c r="D31">
-        <f>POWER(D13,D18)</f>
+        <f t="shared" si="9"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="E31">
-        <f>POWER(E13,E18)</f>
+        <f t="shared" si="9"/>
         <v>1.6875219239328012</v>
       </c>
       <c r="F31">
-        <f>POWER(F13,F18)</f>
+        <f t="shared" si="9"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="G31">
-        <f>POWER(G13,G18)</f>
+        <f t="shared" si="9"/>
         <v>1.9233653142060292</v>
       </c>
       <c r="H31">
-        <f>(B31*C31*D31*E31*F31*G31)</f>
+        <f t="shared" si="0"/>
         <v>34.423083017273157</v>
       </c>
       <c r="J31" t="s">

</xml_diff>